<commit_message>
updated 3 image in single row and comments full inside container
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -397,11 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Urls</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="str">
         <v>https://dev.recordati-plus.de/de_DE/overview-page</v>
@@ -414,7 +419,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A2:A3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Task execution time calculated
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -414,12 +414,57 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-psychiatrie</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-urologie</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
         <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-gastroenterologie</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-psychiatrie</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-paediatrie</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-kardiologie</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-orthopaedie</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-urologie</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-erkaeltung</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-sonstige-praeparate</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All urls included in git
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A388"/>
+  <dimension ref="A1:A439"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,12 +409,1682 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page</v>
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-psychiatrie</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-urologie</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-gastroenterologie</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-psychiatrie</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-paediatrie</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-kardiologie</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-orthopaedie</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-urologie</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-erkaeltung</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-sonstige-praeparate</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/mediathek-urologie</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-orthopaedie</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-paediatrie</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praparate-gastroenterologie-0002</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-gastroenterologie</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-paediatrie</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-kardiologie</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-orthopaedie</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-psychiatrie</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-urologie</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-erkaeltung</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-sonstige</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/akademie</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/mediathek</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-wundheilung</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/recordati-plus-gated</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-urologie-test</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/demo-home</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/overview-page/recordati-plus-home</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/belociv</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/beloc-zok</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/corifeo</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/lercanidipin-omniapharm</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/metoprololtartrat-omniapharm</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/zanipress</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/mobloc</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/betadorm-d</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/citrafleet</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/claversal</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/collomack-topical</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/xitix-lutschtabletten</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/zentramin</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/jhp-rodler-japanisches-minzol</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/rhinopront</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/flosa-balance</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/phospho-soda</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/laxbene-junior</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/mirfulan-wund-und-heilsalbe</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/mirfulan-spray-n</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/mirfulan-hydrolind-creme</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/binosto-brausetabletten</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/dexabene</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/dolobene-ibu</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/lipotalon</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/ortoton</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/osteoplus</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/recosyn</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/reagila</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/eligard</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/fortacin</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/urorec</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/spasuret</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/sportvis</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/ambene-parenteral</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/recosyn-max-forte-n</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/products/test1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/mirfulan-wund-und-heilsalbe</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/rhinopront-kombi-tabletten</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/windeldermatitis-bei-babys-und-kleinkindern</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/dekubitus</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/intertrigo-bei-uebergewicht</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/windeldermatitis-bei-erwachsenen</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-mirfulan-wund-und-heilsalbe</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-mirfulan-spray</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/schnupfenformen</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/nasenspray-abhaengigkeit</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-rhinoPRONT</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/neurodermitis-erkennen</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/mirfulan-salbenspray</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/neurodermitis-behandeln</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/laxbene</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/risiko-melatonin</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/stiftung-warentest</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/elektrolyte</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/erste-wahl-bei-verstopfung</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-betadorm</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-laxbene</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/Wie-die-Zeitumstellung-die-Gesundheit-beeintraechtigt</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/demo-otc</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/mirfulan-hydrolind</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/otc-page/betadorm</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1758</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/35</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/36</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/37</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/38</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/39</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/40</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/41</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/69</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/70</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/71</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/72</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/73</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/74</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/75</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/76</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/77</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/78</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/79</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/80</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/81</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/82</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/83</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/84</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/85</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/86</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/87</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/88</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/89</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/90</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/91</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/92</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/94</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/95</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/96</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/97</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/98</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/99</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/100</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/101</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/102</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/103</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/105</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/107</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/108</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/109</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/110</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/113</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/120</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/135</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/136</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/137</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/172</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/174</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/175</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/176</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/177</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/178</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/179</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/180</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/181</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/182</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/183</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/184</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/186</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/187</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/188</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/189</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/190</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/193</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/194</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/195</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/196</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/197</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/198</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/199</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/208</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/209</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/210</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/211</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/212</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/213</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/214</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/215</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/216</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/217</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/218</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/219</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/220</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/221</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/223</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/227</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/228</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/240</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/242</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/326</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/248</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/251</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/257</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/258</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/259</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/260</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/263</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/265</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/266</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/267</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/268</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/269</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/300</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/301</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/302</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/303</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/304</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/305</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/306</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/307</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/308</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/309</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/310</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/311</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/312</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/313</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/314</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/315</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/316</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/317</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/318</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/319</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/320</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/321</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/322</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/323</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/324</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/325</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/327</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/333</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/366</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/367</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/368</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/369</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/370</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/371</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/372</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/373</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/374</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/375</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/432</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/433</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/434</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/435</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="str">
         <v>https://dev.recordati-plus.de/de_DE/recordati-article/498</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/499</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/500</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/532</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/564</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/565</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/566</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/567</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/568</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/597</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/598</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/632</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/633</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/634</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/635</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/636</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/637</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/638</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/663</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/664</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/665</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/666</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/696</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/729</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/762</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/763</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/764</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/765</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/766</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/767</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/768</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/769</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/795</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/796</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/797</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/828</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/829</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/830</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/861</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/894</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/895</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/896</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/927</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/928</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/929</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/930</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/931</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/932</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/933</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/934</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/935</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/937</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/938</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/939</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/940</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/941</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/942</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/943</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/944</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/945</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/946</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/947</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/948</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/949</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/950</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/960</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/961</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/994</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/995</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1092</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1093</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1094</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1125</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1158</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1191</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1224</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1257</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1258</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1259</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1260</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1261</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1262</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1263</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1264</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1265</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1266</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1267</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1268</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1269</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1270</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="str">
+        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1271</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="str">
+        <v>https://dev.recordati-plus.de/</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="str">
+        <v/>
       </c>
     </row>
     <row r="338">
@@ -672,9 +2342,264 @@
         <v/>
       </c>
     </row>
+    <row r="389">
+      <c r="A389" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A388"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A439"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code with compressed version
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -397,2209 +397,2506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A439"/>
+  <dimension ref="A1:B439"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>URLS</v>
+        <v>loc_x000d_</v>
+      </c>
+      <c r="B1" t="str">
+        <v>loc_x000d_</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-psychiatrie</v>
+        <v>http://localhost:3000/de_DE/otc-page/mirfulan-wund-und-heilsalbe_x000d_</v>
+      </c>
+      <c r="B2" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/mirfulan-wund-und-heilsalbe_x000d_</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-urologie</v>
+        <v>http://localhost:3000/de_DE/otc-page/rhinopront-kombi-tabletten_x000d_</v>
+      </c>
+      <c r="B3" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/rhinopront-kombi-tabletten_x000d_</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-gastroenterologie</v>
+        <v>http://localhost:3000/de_DE/otc-page/mirfulan-hydrolind_x000d_</v>
+      </c>
+      <c r="B4" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/mirfulan-hydrolind_x000d_</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-psychiatrie</v>
+        <v>http://localhost:3000/de_DE/otc-page/windeldermatitis-bei-babys-und-kleinkindern_x000d_</v>
+      </c>
+      <c r="B5" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/windeldermatitis-bei-babys-und-kleinkindern_x000d_</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-paediatrie</v>
+        <v>http://localhost:3000/de_DE/otc-page/dekubitus_x000d_</v>
+      </c>
+      <c r="B6" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/dekubitus_x000d_</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-kardiologie</v>
+      <c r="B7" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/intertrigo-bei-uebergewicht_x000d_</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-orthopaedie</v>
+      <c r="B8" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/windeldermatitis-bei-erwachsenen_x000d_</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-urologie</v>
+      <c r="B9" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/pflichttext-mirfulan-wund-und-heilsalbe_x000d_</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-erkaeltung</v>
+      <c r="B10" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/pflichttext-mirfulan-spray_x000d_</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/alle-inhalte-sonstige-praeparate</v>
+      <c r="B11" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/schnupfenformen_x000d_</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/mediathek-urologie</v>
+      <c r="B12" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/nasenspray-abhaengigkeit_x000d_</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-orthopaedie</v>
+      <c r="B13" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/pflichttext-rhinoPRONT_x000d_</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-paediatrie</v>
+      <c r="B14" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/neurodermitis-erkennen_x000d_</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praparate-gastroenterologie-0002</v>
+      <c r="B15" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/mirfulan-salbenspray_x000d_</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-gastroenterologie</v>
+      <c r="B16" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/neurodermitis-behandeln_x000d_</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-paediatrie</v>
+      <c r="B17" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/betadorm_x000d_</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-kardiologie</v>
+      <c r="B18" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/laxbene_x000d_</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-orthopaedie</v>
+      <c r="B19" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/risiko-melatonin_x000d_</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-psychiatrie</v>
+      <c r="B20" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/stiftung-warentest_x000d_</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-urologie</v>
+      <c r="B21" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/elektrolyte_x000d_</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-erkaeltung</v>
+      <c r="B22" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/erste-wahl-bei-verstopfung_x000d_</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-sonstige</v>
+      <c r="B23" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/pflichttext-betadorm_x000d_</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/akademie</v>
+      <c r="B24" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/pflichttext-laxbene_x000d_</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/mediathek</v>
+      <c r="B25" t="str">
+        <v>http://localhost:3000/de_DE/otc-page/Wie-die-Zeitumstellung-die-Gesundheit-beeintraechtigt_x000d_</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate</v>
+      <c r="B26" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/recordati-plus-home_x000d_</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/praeparate-wundheilung</v>
+      <c r="B27" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/home-psychiatrie_x000d_</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/recordati-plus-gated</v>
+      <c r="B28" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/home-urologie_x000d_</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/home-urologie-test</v>
+      <c r="B29" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-gastroenterologie_x000d_</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/demo-home</v>
+      <c r="B30" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-psychiatrie_x000d_</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/overview-page/recordati-plus-home</v>
+      <c r="B31" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-paediatrie_x000d_</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/belociv</v>
+      <c r="B32" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-kardiologie_x000d_</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/beloc-zok</v>
+      <c r="B33" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-orthopaedie_x000d_</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/corifeo</v>
+      <c r="B34" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-urologie_x000d_</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/lercanidipin-omniapharm</v>
+      <c r="B35" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-erkaeltung_x000d_</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/metoprololtartrat-omniapharm</v>
+      <c r="B36" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/alle-inhalte-sonstige-praeparate_x000d_</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/zanipress</v>
+      <c r="B37" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/mediathek-urologie_x000d_</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/mobloc</v>
+      <c r="B38" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/home-orthopaedie_x000d_</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/betadorm-d</v>
+      <c r="B39" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/home-paediatrie_x000d_</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/citrafleet</v>
+      <c r="B40" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praparate-gastroenterologie-0002_x000d_</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/claversal</v>
+      <c r="B41" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-gastroenterologie_x000d_</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/collomack-topical</v>
+      <c r="B42" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-paediatrie_x000d_</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/xitix-lutschtabletten</v>
+      <c r="B43" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-kardiologie_x000d_</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/zentramin</v>
+      <c r="B44" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-orthopaedie_x000d_</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/jhp-rodler-japanisches-minzol</v>
+      <c r="B45" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-psychiatrie_x000d_</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/rhinopront</v>
+      <c r="B46" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-urologie_x000d_</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/flosa-balance</v>
+      <c r="B47" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-erkaeltung_x000d_</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/phospho-soda</v>
+      <c r="B48" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-sonstige_x000d_</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/laxbene-junior</v>
+      <c r="B49" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/akademie_x000d_</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/mirfulan-wund-und-heilsalbe</v>
+      <c r="B50" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/mediathek_x000d_</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/mirfulan-spray-n</v>
+      <c r="B51" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate_x000d_</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/mirfulan-hydrolind-creme</v>
+      <c r="B52" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/praeparate-wundheilung_x000d_</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/binosto-brausetabletten</v>
+      <c r="B53" t="str">
+        <v>http://localhost:3000/de_DE/overview-page/recordati-plus-gated_x000d_</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/dexabene</v>
+      <c r="B54" t="str">
+        <v>http://localhost:3000/de_DE/products/belociv_x000d_</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/dolobene-ibu</v>
+      <c r="B55" t="str">
+        <v>http://localhost:3000/de_DE/products/beloc-zok_x000d_</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/lipotalon</v>
+      <c r="B56" t="str">
+        <v>http://localhost:3000/de_DE/products/corifeo_x000d_</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/ortoton</v>
+      <c r="B57" t="str">
+        <v>http://localhost:3000/de_DE/products/lercanidipin-omniapharm_x000d_</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/osteoplus</v>
+      <c r="B58" t="str">
+        <v>http://localhost:3000/de_DE/products/metoprololtartrat-omniapharm_x000d_</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/recosyn</v>
+      <c r="B59" t="str">
+        <v>http://localhost:3000/de_DE/products/zanipress_x000d_</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/reagila</v>
+      <c r="B60" t="str">
+        <v>http://localhost:3000/de_DE/products/mobloc_x000d_</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/eligard</v>
+      <c r="B61" t="str">
+        <v>http://localhost:3000/de_DE/products/betadorm-d_x000d_</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/fortacin</v>
+      <c r="B62" t="str">
+        <v>http://localhost:3000/de_DE/products/citrafleet_x000d_</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/urorec</v>
+      <c r="B63" t="str">
+        <v>http://localhost:3000/de_DE/products/claversal_x000d_</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/spasuret</v>
+      <c r="B64" t="str">
+        <v>http://localhost:3000/de_DE/products/collomack-topical_x000d_</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/sportvis</v>
+      <c r="B65" t="str">
+        <v>http://localhost:3000/de_DE/products/xitix-lutschtabletten_x000d_</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/ambene-parenteral</v>
+      <c r="B66" t="str">
+        <v>http://localhost:3000/de_DE/products/zentramin_x000d_</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/recosyn-max-forte-n</v>
+      <c r="B67" t="str">
+        <v>http://localhost:3000/de_DE/products/jhp-rodler-japanisches-minzol_x000d_</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/products/test1</v>
+      <c r="B68" t="str">
+        <v>http://localhost:3000/de_DE/products/rhinopront_x000d_</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/mirfulan-wund-und-heilsalbe</v>
+      <c r="B69" t="str">
+        <v>http://localhost:3000/de_DE/products/flosa-balance_x000d_</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/rhinopront-kombi-tabletten</v>
+      <c r="B70" t="str">
+        <v>http://localhost:3000/de_DE/products/phospho-soda_x000d_</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/windeldermatitis-bei-babys-und-kleinkindern</v>
+      <c r="B71" t="str">
+        <v>http://localhost:3000/de_DE/products/laxbene-junior_x000d_</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/dekubitus</v>
+      <c r="B72" t="str">
+        <v>http://localhost:3000/de_DE/products/mirfulan-wund-und-heilsalbe_x000d_</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/intertrigo-bei-uebergewicht</v>
+      <c r="B73" t="str">
+        <v>http://localhost:3000/de_DE/products/mirfulan-spray-n_x000d_</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/windeldermatitis-bei-erwachsenen</v>
+      <c r="B74" t="str">
+        <v>http://localhost:3000/de_DE/products/mirfulan-hydrolind-creme_x000d_</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-mirfulan-wund-und-heilsalbe</v>
+      <c r="B75" t="str">
+        <v>http://localhost:3000/de_DE/products/binosto-brausetabletten_x000d_</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-mirfulan-spray</v>
+      <c r="B76" t="str">
+        <v>http://localhost:3000/de_DE/products/dexabene_x000d_</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/schnupfenformen</v>
+      <c r="B77" t="str">
+        <v>http://localhost:3000/de_DE/products/dolobene-ibu_x000d_</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/nasenspray-abhaengigkeit</v>
+      <c r="B78" t="str">
+        <v>http://localhost:3000/de_DE/products/lipotalon_x000d_</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-rhinoPRONT</v>
+      <c r="B79" t="str">
+        <v>http://localhost:3000/de_DE/products/ortoton_x000d_</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/neurodermitis-erkennen</v>
+      <c r="B80" t="str">
+        <v>http://localhost:3000/de_DE/products/osteoplus_x000d_</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/mirfulan-salbenspray</v>
+      <c r="B81" t="str">
+        <v>http://localhost:3000/de_DE/products/recosyn_x000d_</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/neurodermitis-behandeln</v>
+      <c r="B82" t="str">
+        <v>http://localhost:3000/de_DE/products/reagila_x000d_</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/laxbene</v>
+      <c r="B83" t="str">
+        <v>http://localhost:3000/de_DE/products/eligard_x000d_</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/risiko-melatonin</v>
+      <c r="B84" t="str">
+        <v>http://localhost:3000/de_DE/products/fortacin_x000d_</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/stiftung-warentest</v>
+      <c r="B85" t="str">
+        <v>http://localhost:3000/de_DE/products/urorec_x000d_</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/elektrolyte</v>
+      <c r="B86" t="str">
+        <v>http://localhost:3000/de_DE/products/spasuret_x000d_</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/erste-wahl-bei-verstopfung</v>
+      <c r="B87" t="str">
+        <v>http://localhost:3000/de_DE/products/sportvis_x000d_</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-betadorm</v>
+      <c r="B88" t="str">
+        <v>http://localhost:3000/de_DE/products/ambene-parenteral_x000d_</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/pflichttext-laxbene</v>
+      <c r="B89" t="str">
+        <v>http://localhost:3000/de_DE/products/recosyn-max-forte-n_x000d_</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/Wie-die-Zeitumstellung-die-Gesundheit-beeintraechtigt</v>
+      <c r="B90" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1866_x000d_</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/demo-otc</v>
+      <c r="B91" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1_x000d_</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/mirfulan-hydrolind</v>
+      <c r="B92" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1867_x000d_</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/otc-page/betadorm</v>
+      <c r="B93" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1868_x000d_</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1758</v>
+      <c r="B94" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1872_x000d_</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1</v>
+      <c r="B95" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1869_x000d_</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/35</v>
+      <c r="B96" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1873_x000d_</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/36</v>
+      <c r="B97" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1870_x000d_</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/37</v>
+      <c r="B98" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1875_x000d_</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/38</v>
+      <c r="B99" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1871_x000d_</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/39</v>
+      <c r="B100" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1874_x000d_</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/40</v>
+      <c r="B101" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/35_x000d_</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/41</v>
+      <c r="B102" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/36_x000d_</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/69</v>
+      <c r="B103" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/38_x000d_</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/70</v>
+      <c r="B104" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/40_x000d_</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/71</v>
+      <c r="B105" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/41_x000d_</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/72</v>
+      <c r="B106" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/69_x000d_</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/73</v>
+      <c r="B107" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/70_x000d_</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/74</v>
+      <c r="B108" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/71_x000d_</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/75</v>
+      <c r="B109" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/72_x000d_</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/76</v>
+      <c r="B110" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/73_x000d_</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/77</v>
+      <c r="B111" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/74_x000d_</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/78</v>
+      <c r="B112" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/75_x000d_</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/79</v>
+      <c r="B113" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/76_x000d_</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/80</v>
+      <c r="B114" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/77_x000d_</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/81</v>
+      <c r="B115" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/78_x000d_</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/82</v>
+      <c r="B116" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/79_x000d_</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/83</v>
+      <c r="B117" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/80_x000d_</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/84</v>
+      <c r="B118" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/81_x000d_</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/85</v>
+      <c r="B119" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/82_x000d_</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/86</v>
+      <c r="B120" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/83_x000d_</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/87</v>
+      <c r="B121" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/84_x000d_</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/88</v>
+      <c r="B122" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/85_x000d_</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/89</v>
+      <c r="B123" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/86_x000d_</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/90</v>
+      <c r="B124" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/87_x000d_</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/91</v>
+      <c r="B125" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/88_x000d_</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/92</v>
+      <c r="B126" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/89_x000d_</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/94</v>
+      <c r="B127" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/90_x000d_</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/95</v>
+      <c r="B128" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/91_x000d_</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/96</v>
+      <c r="B129" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/92_x000d_</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/97</v>
+      <c r="B130" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/94_x000d_</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/98</v>
+      <c r="B131" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/95_x000d_</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/99</v>
+      <c r="B132" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/96_x000d_</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/100</v>
+      <c r="B133" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/97_x000d_</v>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/101</v>
+      <c r="B134" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/98_x000d_</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/102</v>
+      <c r="B135" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/99_x000d_</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/103</v>
+      <c r="B136" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/100_x000d_</v>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/105</v>
+      <c r="B137" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/101_x000d_</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/107</v>
+      <c r="B138" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/102_x000d_</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/108</v>
+      <c r="B139" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/103_x000d_</v>
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/109</v>
+      <c r="B140" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/105_x000d_</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/110</v>
+      <c r="B141" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/107_x000d_</v>
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/113</v>
+      <c r="B142" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/108_x000d_</v>
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/120</v>
+      <c r="B143" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/109_x000d_</v>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/135</v>
+      <c r="B144" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/110_x000d_</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/136</v>
+      <c r="B145" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/113_x000d_</v>
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/137</v>
+      <c r="B146" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/120_x000d_</v>
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/172</v>
+      <c r="B147" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/135_x000d_</v>
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/174</v>
+      <c r="B148" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/136_x000d_</v>
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/175</v>
+      <c r="B149" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/137_x000d_</v>
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/176</v>
+      <c r="B150" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/172_x000d_</v>
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/177</v>
+      <c r="B151" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/174_x000d_</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/178</v>
+      <c r="B152" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/175_x000d_</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/179</v>
+      <c r="B153" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/176_x000d_</v>
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/180</v>
+      <c r="B154" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/177_x000d_</v>
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/181</v>
+      <c r="B155" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/178_x000d_</v>
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/182</v>
+      <c r="B156" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/179_x000d_</v>
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/183</v>
+      <c r="B157" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/180_x000d_</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/184</v>
+      <c r="B158" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/181_x000d_</v>
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/186</v>
+      <c r="B159" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/182_x000d_</v>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/187</v>
+      <c r="B160" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/183_x000d_</v>
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/188</v>
+      <c r="B161" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/184_x000d_</v>
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/189</v>
+      <c r="B162" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/186_x000d_</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/190</v>
+      <c r="B163" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/187_x000d_</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/193</v>
+      <c r="B164" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/188_x000d_</v>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/194</v>
+      <c r="B165" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/189_x000d_</v>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/195</v>
+      <c r="B166" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/190_x000d_</v>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/196</v>
+      <c r="B167" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/193_x000d_</v>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/197</v>
+      <c r="B168" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/194_x000d_</v>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/198</v>
+      <c r="B169" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/195_x000d_</v>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/199</v>
+      <c r="B170" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/196_x000d_</v>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/208</v>
+      <c r="B171" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/197_x000d_</v>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/209</v>
+      <c r="B172" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/198_x000d_</v>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/210</v>
+      <c r="B173" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/199_x000d_</v>
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/211</v>
+      <c r="B174" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/208_x000d_</v>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/212</v>
+      <c r="B175" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/209_x000d_</v>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/213</v>
+      <c r="B176" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/210_x000d_</v>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/214</v>
+      <c r="B177" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/211_x000d_</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/215</v>
+      <c r="B178" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/212_x000d_</v>
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/216</v>
+      <c r="B179" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/219_x000d_</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/217</v>
+      <c r="B180" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/221_x000d_</v>
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/218</v>
+      <c r="B181" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/227_x000d_</v>
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/219</v>
+      <c r="B182" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/228_x000d_</v>
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/220</v>
+      <c r="B183" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/240_x000d_</v>
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/221</v>
+      <c r="B184" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/242_x000d_</v>
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/223</v>
+      <c r="B185" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/248_x000d_</v>
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/227</v>
+      <c r="B186" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/251_x000d_</v>
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/228</v>
+      <c r="B187" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/257_x000d_</v>
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/240</v>
+      <c r="B188" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/258_x000d_</v>
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/242</v>
+      <c r="B189" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/259_x000d_</v>
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/326</v>
+      <c r="B190" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/260_x000d_</v>
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/248</v>
+      <c r="B191" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/263_x000d_</v>
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/251</v>
+      <c r="B192" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/265_x000d_</v>
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/257</v>
+      <c r="B193" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/266_x000d_</v>
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/258</v>
+      <c r="B194" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/268_x000d_</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/259</v>
+      <c r="B195" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/269_x000d_</v>
       </c>
     </row>
     <row r="196">
-      <c r="A196" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/260</v>
+      <c r="B196" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/300_x000d_</v>
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/263</v>
+      <c r="B197" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/301_x000d_</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/265</v>
+      <c r="B198" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/303_x000d_</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/266</v>
+      <c r="B199" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/304_x000d_</v>
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/267</v>
+      <c r="B200" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/305_x000d_</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/268</v>
+      <c r="B201" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/306_x000d_</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/269</v>
+      <c r="B202" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/307_x000d_</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/300</v>
+      <c r="B203" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/308_x000d_</v>
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/301</v>
+      <c r="B204" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/309_x000d_</v>
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/302</v>
+      <c r="B205" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/310_x000d_</v>
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/303</v>
+      <c r="B206" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/311_x000d_</v>
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/304</v>
+      <c r="B207" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/312_x000d_</v>
       </c>
     </row>
     <row r="208">
-      <c r="A208" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/305</v>
+      <c r="B208" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/313_x000d_</v>
       </c>
     </row>
     <row r="209">
-      <c r="A209" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/306</v>
+      <c r="B209" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/314_x000d_</v>
       </c>
     </row>
     <row r="210">
-      <c r="A210" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/307</v>
+      <c r="B210" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/315_x000d_</v>
       </c>
     </row>
     <row r="211">
-      <c r="A211" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/308</v>
+      <c r="B211" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/316_x000d_</v>
       </c>
     </row>
     <row r="212">
-      <c r="A212" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/309</v>
+      <c r="B212" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/317_x000d_</v>
       </c>
     </row>
     <row r="213">
-      <c r="A213" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/310</v>
+      <c r="B213" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/318_x000d_</v>
       </c>
     </row>
     <row r="214">
-      <c r="A214" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/311</v>
+      <c r="B214" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/319_x000d_</v>
       </c>
     </row>
     <row r="215">
-      <c r="A215" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/312</v>
+      <c r="B215" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/320_x000d_</v>
       </c>
     </row>
     <row r="216">
-      <c r="A216" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/313</v>
+      <c r="B216" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/321_x000d_</v>
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/314</v>
+      <c r="B217" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/322_x000d_</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/315</v>
+      <c r="B218" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/323_x000d_</v>
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/316</v>
+      <c r="B219" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/324_x000d_</v>
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/317</v>
+      <c r="B220" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/325_x000d_</v>
       </c>
     </row>
     <row r="221">
-      <c r="A221" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/318</v>
+      <c r="B221" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/333_x000d_</v>
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/319</v>
+      <c r="B222" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/366_x000d_</v>
       </c>
     </row>
     <row r="223">
-      <c r="A223" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/320</v>
+      <c r="B223" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/367_x000d_</v>
       </c>
     </row>
     <row r="224">
-      <c r="A224" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/321</v>
+      <c r="B224" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/368_x000d_</v>
       </c>
     </row>
     <row r="225">
-      <c r="A225" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/322</v>
+      <c r="B225" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/369_x000d_</v>
       </c>
     </row>
     <row r="226">
-      <c r="A226" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/323</v>
+      <c r="B226" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/370_x000d_</v>
       </c>
     </row>
     <row r="227">
-      <c r="A227" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/324</v>
+      <c r="B227" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/371_x000d_</v>
       </c>
     </row>
     <row r="228">
-      <c r="A228" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/325</v>
+      <c r="B228" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/372_x000d_</v>
       </c>
     </row>
     <row r="229">
-      <c r="A229" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/327</v>
+      <c r="B229" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/373_x000d_</v>
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/333</v>
+      <c r="B230" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/374_x000d_</v>
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/366</v>
+      <c r="B231" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/375_x000d_</v>
       </c>
     </row>
     <row r="232">
-      <c r="A232" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/367</v>
+      <c r="B232" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/432_x000d_</v>
       </c>
     </row>
     <row r="233">
-      <c r="A233" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/368</v>
+      <c r="B233" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/433_x000d_</v>
       </c>
     </row>
     <row r="234">
-      <c r="A234" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/369</v>
+      <c r="B234" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/434_x000d_</v>
       </c>
     </row>
     <row r="235">
-      <c r="A235" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/370</v>
+      <c r="B235" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/435_x000d_</v>
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/371</v>
+      <c r="B236" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/498_x000d_</v>
       </c>
     </row>
     <row r="237">
-      <c r="A237" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/372</v>
+      <c r="B237" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/499_x000d_</v>
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/373</v>
+      <c r="B238" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/500_x000d_</v>
       </c>
     </row>
     <row r="239">
-      <c r="A239" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/374</v>
+      <c r="B239" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/532_x000d_</v>
       </c>
     </row>
     <row r="240">
-      <c r="A240" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/375</v>
+      <c r="B240" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/564_x000d_</v>
       </c>
     </row>
     <row r="241">
-      <c r="A241" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/432</v>
+      <c r="B241" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/565_x000d_</v>
       </c>
     </row>
     <row r="242">
-      <c r="A242" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/433</v>
+      <c r="B242" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/566_x000d_</v>
       </c>
     </row>
     <row r="243">
-      <c r="A243" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/434</v>
+      <c r="B243" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/567_x000d_</v>
       </c>
     </row>
     <row r="244">
-      <c r="A244" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/435</v>
+      <c r="B244" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/568_x000d_</v>
       </c>
     </row>
     <row r="245">
-      <c r="A245" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/498</v>
+      <c r="B245" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/597_x000d_</v>
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/499</v>
+      <c r="B246" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/598_x000d_</v>
       </c>
     </row>
     <row r="247">
-      <c r="A247" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/500</v>
+      <c r="B247" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/632_x000d_</v>
       </c>
     </row>
     <row r="248">
-      <c r="A248" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/532</v>
+      <c r="B248" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/633_x000d_</v>
       </c>
     </row>
     <row r="249">
-      <c r="A249" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/564</v>
+      <c r="B249" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/634_x000d_</v>
       </c>
     </row>
     <row r="250">
-      <c r="A250" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/565</v>
+      <c r="B250" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/635_x000d_</v>
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/566</v>
+      <c r="B251" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/636_x000d_</v>
       </c>
     </row>
     <row r="252">
-      <c r="A252" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/567</v>
+      <c r="B252" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/637_x000d_</v>
       </c>
     </row>
     <row r="253">
-      <c r="A253" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/568</v>
+      <c r="B253" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/638_x000d_</v>
       </c>
     </row>
     <row r="254">
-      <c r="A254" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/597</v>
+      <c r="B254" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/663_x000d_</v>
       </c>
     </row>
     <row r="255">
-      <c r="A255" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/598</v>
+      <c r="B255" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/664_x000d_</v>
       </c>
     </row>
     <row r="256">
-      <c r="A256" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/632</v>
+      <c r="B256" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/665_x000d_</v>
       </c>
     </row>
     <row r="257">
-      <c r="A257" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/633</v>
+      <c r="B257" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/666_x000d_</v>
       </c>
     </row>
     <row r="258">
-      <c r="A258" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/634</v>
+      <c r="B258" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/696_x000d_</v>
       </c>
     </row>
     <row r="259">
-      <c r="A259" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/635</v>
+      <c r="B259" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/729_x000d_</v>
       </c>
     </row>
     <row r="260">
-      <c r="A260" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/636</v>
+      <c r="B260" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/762_x000d_</v>
       </c>
     </row>
     <row r="261">
-      <c r="A261" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/637</v>
+      <c r="B261" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/763_x000d_</v>
       </c>
     </row>
     <row r="262">
-      <c r="A262" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/638</v>
+      <c r="B262" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/764_x000d_</v>
       </c>
     </row>
     <row r="263">
-      <c r="A263" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/663</v>
+      <c r="B263" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/765_x000d_</v>
       </c>
     </row>
     <row r="264">
-      <c r="A264" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/664</v>
+      <c r="B264" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/949_x000d_</v>
       </c>
     </row>
     <row r="265">
-      <c r="A265" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/665</v>
+      <c r="B265" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/766_x000d_</v>
       </c>
     </row>
     <row r="266">
-      <c r="A266" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/666</v>
+      <c r="B266" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/767_x000d_</v>
       </c>
     </row>
     <row r="267">
-      <c r="A267" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/696</v>
+      <c r="B267" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/768_x000d_</v>
       </c>
     </row>
     <row r="268">
-      <c r="A268" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/729</v>
+      <c r="B268" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/769_x000d_</v>
       </c>
     </row>
     <row r="269">
-      <c r="A269" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/762</v>
+      <c r="B269" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/795_x000d_</v>
       </c>
     </row>
     <row r="270">
-      <c r="A270" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/763</v>
+      <c r="B270" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/796_x000d_</v>
       </c>
     </row>
     <row r="271">
-      <c r="A271" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/764</v>
+      <c r="B271" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/797_x000d_</v>
       </c>
     </row>
     <row r="272">
-      <c r="A272" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/765</v>
+      <c r="B272" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/828_x000d_</v>
       </c>
     </row>
     <row r="273">
-      <c r="A273" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/766</v>
+      <c r="B273" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/829_x000d_</v>
       </c>
     </row>
     <row r="274">
-      <c r="A274" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/767</v>
+      <c r="B274" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/830_x000d_</v>
       </c>
     </row>
     <row r="275">
-      <c r="A275" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/768</v>
+      <c r="B275" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/861_x000d_</v>
       </c>
     </row>
     <row r="276">
-      <c r="A276" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/769</v>
+      <c r="B276" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/894_x000d_</v>
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/795</v>
+      <c r="B277" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/895_x000d_</v>
       </c>
     </row>
     <row r="278">
-      <c r="A278" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/796</v>
+      <c r="B278" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/896_x000d_</v>
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/797</v>
+      <c r="B279" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/927_x000d_</v>
       </c>
     </row>
     <row r="280">
-      <c r="A280" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/828</v>
+      <c r="B280" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/928_x000d_</v>
       </c>
     </row>
     <row r="281">
-      <c r="A281" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/829</v>
+      <c r="B281" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/929_x000d_</v>
       </c>
     </row>
     <row r="282">
-      <c r="A282" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/830</v>
+      <c r="B282" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/930_x000d_</v>
       </c>
     </row>
     <row r="283">
-      <c r="A283" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/861</v>
+      <c r="B283" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/931_x000d_</v>
       </c>
     </row>
     <row r="284">
-      <c r="A284" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/894</v>
+      <c r="B284" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/932_x000d_</v>
       </c>
     </row>
     <row r="285">
-      <c r="A285" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/895</v>
+      <c r="B285" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/933_x000d_</v>
       </c>
     </row>
     <row r="286">
-      <c r="A286" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/896</v>
+      <c r="B286" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/934_x000d_</v>
       </c>
     </row>
     <row r="287">
-      <c r="A287" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/927</v>
+      <c r="B287" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/935_x000d_</v>
       </c>
     </row>
     <row r="288">
-      <c r="A288" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/928</v>
+      <c r="B288" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/937_x000d_</v>
       </c>
     </row>
     <row r="289">
-      <c r="A289" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/929</v>
+      <c r="B289" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/938_x000d_</v>
       </c>
     </row>
     <row r="290">
-      <c r="A290" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/930</v>
+      <c r="B290" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/939_x000d_</v>
       </c>
     </row>
     <row r="291">
-      <c r="A291" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/931</v>
+      <c r="B291" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/940_x000d_</v>
       </c>
     </row>
     <row r="292">
-      <c r="A292" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/932</v>
+      <c r="B292" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/941_x000d_</v>
       </c>
     </row>
     <row r="293">
-      <c r="A293" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/933</v>
+      <c r="B293" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/942_x000d_</v>
       </c>
     </row>
     <row r="294">
-      <c r="A294" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/934</v>
+      <c r="B294" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/943_x000d_</v>
       </c>
     </row>
     <row r="295">
-      <c r="A295" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/935</v>
+      <c r="B295" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/944_x000d_</v>
       </c>
     </row>
     <row r="296">
-      <c r="A296" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/937</v>
+      <c r="B296" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/945_x000d_</v>
       </c>
     </row>
     <row r="297">
-      <c r="A297" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/938</v>
+      <c r="B297" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/946_x000d_</v>
       </c>
     </row>
     <row r="298">
-      <c r="A298" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/939</v>
+      <c r="B298" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/947_x000d_</v>
       </c>
     </row>
     <row r="299">
-      <c r="A299" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/940</v>
+      <c r="B299" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/948_x000d_</v>
       </c>
     </row>
     <row r="300">
-      <c r="A300" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/941</v>
+      <c r="B300" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/950_x000d_</v>
       </c>
     </row>
     <row r="301">
-      <c r="A301" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/942</v>
+      <c r="B301" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/960_x000d_</v>
       </c>
     </row>
     <row r="302">
-      <c r="A302" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/943</v>
+      <c r="B302" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/961_x000d_</v>
       </c>
     </row>
     <row r="303">
-      <c r="A303" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/944</v>
+      <c r="B303" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/994_x000d_</v>
       </c>
     </row>
     <row r="304">
-      <c r="A304" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/945</v>
+      <c r="B304" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/995_x000d_</v>
       </c>
     </row>
     <row r="305">
-      <c r="A305" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/946</v>
+      <c r="B305" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1092_x000d_</v>
       </c>
     </row>
     <row r="306">
-      <c r="A306" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/947</v>
+      <c r="B306" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1093_x000d_</v>
       </c>
     </row>
     <row r="307">
-      <c r="A307" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/948</v>
+      <c r="B307" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1094_x000d_</v>
       </c>
     </row>
     <row r="308">
-      <c r="A308" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/949</v>
+      <c r="B308" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1125_x000d_</v>
       </c>
     </row>
     <row r="309">
-      <c r="A309" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/950</v>
+      <c r="B309" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1191_x000d_</v>
       </c>
     </row>
     <row r="310">
-      <c r="A310" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/960</v>
+      <c r="B310" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1224_x000d_</v>
       </c>
     </row>
     <row r="311">
-      <c r="A311" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/961</v>
+      <c r="B311" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1257_x000d_</v>
       </c>
     </row>
     <row r="312">
-      <c r="A312" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/994</v>
+      <c r="B312" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1258_x000d_</v>
       </c>
     </row>
     <row r="313">
-      <c r="A313" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/995</v>
+      <c r="B313" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1259_x000d_</v>
       </c>
     </row>
     <row r="314">
-      <c r="A314" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1092</v>
+      <c r="B314" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1260_x000d_</v>
       </c>
     </row>
     <row r="315">
-      <c r="A315" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1093</v>
+      <c r="B315" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1261_x000d_</v>
       </c>
     </row>
     <row r="316">
-      <c r="A316" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1094</v>
+      <c r="B316" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1262_x000d_</v>
       </c>
     </row>
     <row r="317">
-      <c r="A317" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1125</v>
+      <c r="B317" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1263_x000d_</v>
       </c>
     </row>
     <row r="318">
-      <c r="A318" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1158</v>
+      <c r="B318" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1264_x000d_</v>
       </c>
     </row>
     <row r="319">
-      <c r="A319" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1191</v>
+      <c r="B319" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1265_x000d_</v>
       </c>
     </row>
     <row r="320">
-      <c r="A320" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1224</v>
+      <c r="B320" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1266_x000d_</v>
       </c>
     </row>
     <row r="321">
-      <c r="A321" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1257</v>
+      <c r="B321" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1267_x000d_</v>
       </c>
     </row>
     <row r="322">
-      <c r="A322" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1258</v>
+      <c r="B322" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1268_x000d_</v>
       </c>
     </row>
     <row r="323">
-      <c r="A323" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1259</v>
+      <c r="B323" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1269_x000d_</v>
       </c>
     </row>
     <row r="324">
-      <c r="A324" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1260</v>
+      <c r="B324" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1270_x000d_</v>
       </c>
     </row>
     <row r="325">
-      <c r="A325" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1261</v>
+      <c r="B325" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1271_x000d_</v>
       </c>
     </row>
     <row r="326">
-      <c r="A326" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1262</v>
+      <c r="B326" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1272_x000d_</v>
       </c>
     </row>
     <row r="327">
-      <c r="A327" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1263</v>
+      <c r="B327" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1273_x000d_</v>
       </c>
     </row>
     <row r="328">
-      <c r="A328" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1264</v>
+      <c r="B328" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1274_x000d_</v>
       </c>
     </row>
     <row r="329">
-      <c r="A329" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1265</v>
+      <c r="B329" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1275_x000d_</v>
       </c>
     </row>
     <row r="330">
-      <c r="A330" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1266</v>
+      <c r="B330" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1276_x000d_</v>
       </c>
     </row>
     <row r="331">
-      <c r="A331" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1267</v>
+      <c r="B331" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1277_x000d_</v>
       </c>
     </row>
     <row r="332">
-      <c r="A332" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1268</v>
+      <c r="B332" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1278_x000d_</v>
       </c>
     </row>
     <row r="333">
-      <c r="A333" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1269</v>
+      <c r="B333" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1279_x000d_</v>
       </c>
     </row>
     <row r="334">
-      <c r="A334" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1270</v>
+      <c r="B334" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1280_x000d_</v>
       </c>
     </row>
     <row r="335">
-      <c r="A335" t="str">
-        <v>https://dev.recordati-plus.de/de_DE/recordati-article/1271</v>
+      <c r="B335" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1281_x000d_</v>
       </c>
     </row>
     <row r="336">
-      <c r="A336" t="str">
-        <v>https://dev.recordati-plus.de/</v>
+      <c r="B336" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1282_x000d_</v>
       </c>
     </row>
     <row r="337">
-      <c r="A337" t="str">
-        <v/>
+      <c r="B337" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1283_x000d_</v>
       </c>
     </row>
     <row r="338">
-      <c r="A338" t="str">
-        <v/>
+      <c r="B338" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1285_x000d_</v>
       </c>
     </row>
     <row r="339">
-      <c r="A339" t="str">
-        <v/>
+      <c r="B339" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1286_x000d_</v>
       </c>
     </row>
     <row r="340">
-      <c r="A340" t="str">
-        <v/>
+      <c r="B340" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1287_x000d_</v>
       </c>
     </row>
     <row r="341">
-      <c r="A341" t="str">
-        <v/>
+      <c r="B341" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1288_x000d_</v>
       </c>
     </row>
     <row r="342">
-      <c r="A342" t="str">
-        <v/>
+      <c r="B342" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1346_x000d_</v>
       </c>
     </row>
     <row r="343">
-      <c r="A343" t="str">
-        <v/>
+      <c r="B343" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1347_x000d_</v>
       </c>
     </row>
     <row r="344">
-      <c r="A344" t="str">
-        <v/>
+      <c r="B344" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1348_x000d_</v>
       </c>
     </row>
     <row r="345">
-      <c r="A345" t="str">
-        <v/>
+      <c r="B345" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1349_x000d_</v>
       </c>
     </row>
     <row r="346">
-      <c r="A346" t="str">
-        <v/>
+      <c r="B346" t="str">
+        <v>http://localhost:3000/de_DE/recordati-article/1350</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
         <v/>
       </c>
+      <c r="B347" t="str">
+        <v/>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
         <v/>
       </c>
+      <c r="B348" t="str">
+        <v/>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
         <v/>
       </c>
+      <c r="B349" t="str">
+        <v/>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
         <v/>
       </c>
+      <c r="B350" t="str">
+        <v/>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
         <v/>
       </c>
+      <c r="B351" t="str">
+        <v/>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
         <v/>
       </c>
+      <c r="B352" t="str">
+        <v/>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
         <v/>
       </c>
+      <c r="B353" t="str">
+        <v/>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
         <v/>
       </c>
+      <c r="B354" t="str">
+        <v/>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
         <v/>
       </c>
+      <c r="B355" t="str">
+        <v/>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
         <v/>
       </c>
+      <c r="B356" t="str">
+        <v/>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
         <v/>
       </c>
+      <c r="B357" t="str">
+        <v/>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
         <v/>
       </c>
+      <c r="B358" t="str">
+        <v/>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
         <v/>
       </c>
+      <c r="B359" t="str">
+        <v/>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
         <v/>
       </c>
+      <c r="B360" t="str">
+        <v/>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
         <v/>
       </c>
+      <c r="B361" t="str">
+        <v/>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
         <v/>
       </c>
+      <c r="B362" t="str">
+        <v/>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
         <v/>
       </c>
+      <c r="B363" t="str">
+        <v/>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
         <v/>
       </c>
+      <c r="B364" t="str">
+        <v/>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
         <v/>
       </c>
+      <c r="B365" t="str">
+        <v/>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
         <v/>
       </c>
+      <c r="B366" t="str">
+        <v/>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
         <v/>
       </c>
+      <c r="B367" t="str">
+        <v/>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
         <v/>
       </c>
+      <c r="B368" t="str">
+        <v/>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
         <v/>
       </c>
+      <c r="B369" t="str">
+        <v/>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
         <v/>
       </c>
+      <c r="B370" t="str">
+        <v/>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
         <v/>
       </c>
+      <c r="B371" t="str">
+        <v/>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
         <v/>
       </c>
+      <c r="B372" t="str">
+        <v/>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
         <v/>
       </c>
+      <c r="B373" t="str">
+        <v/>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
         <v/>
       </c>
+      <c r="B374" t="str">
+        <v/>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
         <v/>
       </c>
+      <c r="B375" t="str">
+        <v/>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
         <v/>
       </c>
+      <c r="B376" t="str">
+        <v/>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
         <v/>
       </c>
+      <c r="B377" t="str">
+        <v/>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
         <v/>
       </c>
+      <c r="B378" t="str">
+        <v/>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
         <v/>
       </c>
+      <c r="B379" t="str">
+        <v/>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
         <v/>
       </c>
+      <c r="B380" t="str">
+        <v/>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
         <v/>
       </c>
+      <c r="B381" t="str">
+        <v/>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
         <v/>
       </c>
+      <c r="B382" t="str">
+        <v/>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
         <v/>
       </c>
+      <c r="B383" t="str">
+        <v/>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
         <v/>
       </c>
+      <c r="B384" t="str">
+        <v/>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
         <v/>
       </c>
+      <c r="B385" t="str">
+        <v/>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
         <v/>
       </c>
+      <c r="B386" t="str">
+        <v/>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
         <v/>
       </c>
+      <c r="B387" t="str">
+        <v/>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
         <v/>
       </c>
+      <c r="B388" t="str">
+        <v/>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
         <v/>
       </c>
+      <c r="B389" t="str">
+        <v/>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
         <v/>
       </c>
+      <c r="B390" t="str">
+        <v/>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
         <v/>
       </c>
+      <c r="B391" t="str">
+        <v/>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
         <v/>
       </c>
+      <c r="B392" t="str">
+        <v/>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
         <v/>
       </c>
+      <c r="B393" t="str">
+        <v/>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
         <v/>
       </c>
+      <c r="B394" t="str">
+        <v/>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
         <v/>
       </c>
+      <c r="B395" t="str">
+        <v/>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
         <v/>
       </c>
+      <c r="B396" t="str">
+        <v/>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
         <v/>
       </c>
+      <c r="B397" t="str">
+        <v/>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
         <v/>
       </c>
+      <c r="B398" t="str">
+        <v/>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
         <v/>
       </c>
+      <c r="B399" t="str">
+        <v/>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
         <v/>
       </c>
+      <c r="B400" t="str">
+        <v/>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
         <v/>
       </c>
+      <c r="B401" t="str">
+        <v/>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
         <v/>
       </c>
+      <c r="B402" t="str">
+        <v/>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
         <v/>
       </c>
+      <c r="B403" t="str">
+        <v/>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
         <v/>
       </c>
+      <c r="B404" t="str">
+        <v/>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
         <v/>
       </c>
+      <c r="B405" t="str">
+        <v/>
+      </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
         <v/>
       </c>
+      <c r="B406" t="str">
+        <v/>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
         <v/>
       </c>
+      <c r="B407" t="str">
+        <v/>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
         <v/>
       </c>
+      <c r="B408" t="str">
+        <v/>
+      </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
         <v/>
       </c>
+      <c r="B409" t="str">
+        <v/>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
         <v/>
       </c>
+      <c r="B410" t="str">
+        <v/>
+      </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
         <v/>
       </c>
+      <c r="B411" t="str">
+        <v/>
+      </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
         <v/>
       </c>
+      <c r="B412" t="str">
+        <v/>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
         <v/>
       </c>
+      <c r="B413" t="str">
+        <v/>
+      </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
         <v/>
       </c>
+      <c r="B414" t="str">
+        <v/>
+      </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
         <v/>
       </c>
+      <c r="B415" t="str">
+        <v/>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
         <v/>
       </c>
+      <c r="B416" t="str">
+        <v/>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
         <v/>
       </c>
+      <c r="B417" t="str">
+        <v/>
+      </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
         <v/>
       </c>
+      <c r="B418" t="str">
+        <v/>
+      </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
         <v/>
       </c>
+      <c r="B419" t="str">
+        <v/>
+      </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
         <v/>
       </c>
+      <c r="B420" t="str">
+        <v/>
+      </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
         <v/>
       </c>
+      <c r="B421" t="str">
+        <v/>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
         <v/>
       </c>
+      <c r="B422" t="str">
+        <v/>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
         <v/>
       </c>
+      <c r="B423" t="str">
+        <v/>
+      </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
         <v/>
       </c>
+      <c r="B424" t="str">
+        <v/>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
         <v/>
       </c>
+      <c r="B425" t="str">
+        <v/>
+      </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
         <v/>
       </c>
+      <c r="B426" t="str">
+        <v/>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
         <v/>
       </c>
+      <c r="B427" t="str">
+        <v/>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
         <v/>
       </c>
+      <c r="B428" t="str">
+        <v/>
+      </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
         <v/>
       </c>
+      <c r="B429" t="str">
+        <v/>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
         <v/>
       </c>
+      <c r="B430" t="str">
+        <v/>
+      </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
         <v/>
       </c>
+      <c r="B431" t="str">
+        <v/>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
         <v/>
       </c>
+      <c r="B432" t="str">
+        <v/>
+      </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
         <v/>
       </c>
+      <c r="B433" t="str">
+        <v/>
+      </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
         <v/>
       </c>
+      <c r="B434" t="str">
+        <v/>
+      </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
         <v/>
       </c>
+      <c r="B435" t="str">
+        <v/>
+      </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
         <v/>
       </c>
+      <c r="B436" t="str">
+        <v/>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
         <v/>
       </c>
+      <c r="B437" t="str">
+        <v/>
+      </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
         <v/>
       </c>
+      <c r="B438" t="str">
+        <v/>
+      </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
         <v/>
       </c>
+      <c r="B439" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A439"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B439"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>